<commit_message>
update in script excelResultHighPriorityBugV2.1.11_K.xlsx
</commit_message>
<xml_diff>
--- a/Library/HighPriorityBugExcel/excelResultHighPriorityBugV2.1.11_K.xlsx
+++ b/Library/HighPriorityBugExcel/excelResultHighPriorityBugV2.1.11_K.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="77">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -628,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1188,7 +1188,9 @@
         <v>34</v>
       </c>
       <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
+      <c r="G25" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="H25" s="2" t="s">
         <v>75</v>
       </c>
@@ -1442,7 +1444,9 @@
         <v>34</v>
       </c>
       <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
+      <c r="G37" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="H37" s="2" t="s">
         <v>75</v>
       </c>
@@ -1464,7 +1468,9 @@
         <v>10</v>
       </c>
       <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
+      <c r="G38" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="H38" s="2" t="s">
         <v>75</v>
       </c>
@@ -1486,7 +1492,9 @@
         <v>13</v>
       </c>
       <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
+      <c r="G39" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="H39" s="2" t="s">
         <v>75</v>
       </c>
@@ -1508,7 +1516,9 @@
         <v>15</v>
       </c>
       <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
+      <c r="G40" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="H40" s="2" t="s">
         <v>75</v>
       </c>
@@ -1530,7 +1540,9 @@
         <v>17</v>
       </c>
       <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
+      <c r="G41" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="H41" s="2" t="s">
         <v>75</v>
       </c>

</xml_diff>